<commit_message>
first launch of runhaag; verification ongoing. Some bugs found + fixed
</commit_message>
<xml_diff>
--- a/data/haag/haag.xlsx
+++ b/data/haag/haag.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
   <si>
     <t>Commodity</t>
   </si>
@@ -312,12 +312,6 @@
     <t>In Richter: GT (gas turbine), DT (steam turbine), so maybe split into two processes as well</t>
   </si>
   <si>
-    <t>In Richter: MV</t>
-  </si>
-  <si>
-    <t>In Richter: BK</t>
-  </si>
-  <si>
     <t>not mentioned</t>
   </si>
   <si>
@@ -327,10 +321,19 @@
     <t>Waste</t>
   </si>
   <si>
-    <t>not mentioned (interesting: why?)</t>
-  </si>
-  <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>not mentioned in Richter</t>
+  </si>
+  <si>
+    <t>not mentioned in Richter (interesting: why?)</t>
+  </si>
+  <si>
+    <t>in Richter: BK</t>
+  </si>
+  <si>
+    <t>in Richter: MV</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1288,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1464,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1501,11 +1504,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1540,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1583,7 +1586,7 @@
         <v>600000</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1606,7 +1609,7 @@
         <v>800</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1614,10 +1617,10 @@
         <v>66</v>
       </c>
       <c r="B5" s="38">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -1629,7 +1632,7 @@
         <v>150000</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1675,7 +1678,7 @@
         <v>99999</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1698,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1721,11 +1724,11 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="D1"/>
@@ -2069,7 +2072,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2178,7 +2181,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,7 +2337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>